<commit_message>
DataDrivenTest OK quitting driver
</commit_message>
<xml_diff>
--- a/testdata/testData.xlsx
+++ b/testdata/testData.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cesar\git\repository\seleniumAuto\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C3CB332-9924-482C-B7E1-80EB9D69D95B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDB767F0-9AE4-4BBA-BF96-BEA69B134842}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="14">
   <si>
     <t>Principle</t>
   </si>
@@ -149,10 +149,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -452,17 +452,17 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="H2" sqref="H2:H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="8.85546875"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="14.85546875"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="14.7109375"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="13.85546875"/>
+    <col min="7" max="7" customWidth="true" width="13.0"/>
+    <col min="8" max="8" customWidth="true" width="13.42578125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -472,10 +472,10 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6"/>
+      <c r="D1" s="7"/>
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
@@ -511,7 +511,7 @@
       <c r="G2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" t="s" s="0">
         <v>13</v>
       </c>
     </row>
@@ -537,7 +537,7 @@
       <c r="G3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" t="s" s="0">
         <v>13</v>
       </c>
     </row>
@@ -563,7 +563,7 @@
       <c r="G4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="H4" t="s" s="0">
         <v>13</v>
       </c>
     </row>
@@ -589,7 +589,7 @@
       <c r="G5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" t="s" s="0">
         <v>13</v>
       </c>
     </row>
@@ -615,7 +615,7 @@
       <c r="G6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" t="s" s="0">
         <v>8</v>
       </c>
     </row>

</xml_diff>